<commit_message>
Working on building stock generator and see whats happend with will
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/energy_fact_file_housing_stock_age.xlsx
+++ b/data/residential_model/_EXCELFILES/energy_fact_file_housing_stock_age.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="135" windowWidth="23955" windowHeight="8760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="data_prepared" sheetId="2" r:id="rId1"/>
+    <sheet name="original_data" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,30 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>YEAR</t>
-  </si>
-  <si>
-    <t>SEMI_DETACHED</t>
-  </si>
-  <si>
-    <t>TERRACED</t>
-  </si>
-  <si>
-    <t>FLAT</t>
-  </si>
-  <si>
-    <t>DETACHED</t>
-  </si>
-  <si>
-    <t>BUNGALOW</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
 </sst>
 </file>
@@ -64,7 +43,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,16 +257,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -311,7 +290,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10077450" y="333375"/>
+          <a:off x="8734425" y="0"/>
           <a:ext cx="6648450" cy="6905625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -621,10 +600,1099 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1918</v>
+      </c>
+      <c r="C1">
+        <f>(1918+1938)/2</f>
+        <v>1928</v>
+      </c>
+      <c r="D1">
+        <f>(1939+1959)/2</f>
+        <v>1949</v>
+      </c>
+      <c r="E1">
+        <f>ROUND((1960+1975)/2,0)</f>
+        <v>1968</v>
+      </c>
+      <c r="F1">
+        <f>ROUND((1976+2015)/2,2)</f>
+        <v>1995.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1970</v>
+      </c>
+      <c r="B2">
+        <f>(100/SUM(original_data!$B2:$F2))*original_data!B2</f>
+        <v>12.733000787608297</v>
+      </c>
+      <c r="C2">
+        <f>(100/SUM(original_data!$B2:$F2))*original_data!C2</f>
+        <v>13.599369913363088</v>
+      </c>
+      <c r="D2">
+        <f>(100/SUM(original_data!$B2:$F2))*original_data!D2</f>
+        <v>13.153058545550014</v>
+      </c>
+      <c r="E2">
+        <f>(100/SUM(original_data!$B2:$F2))*original_data!E2</f>
+        <v>10.527697558414284</v>
+      </c>
+      <c r="F2">
+        <f>(100/SUM(original_data!$B2:$F2))*original_data!F2</f>
+        <v>49.986873195064327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1971</v>
+      </c>
+      <c r="B3">
+        <f>(100/SUM(original_data!$B3:$F3))*original_data!B3</f>
+        <v>12.279335410176531</v>
+      </c>
+      <c r="C3">
+        <f>(100/SUM(original_data!$B3:$F3))*original_data!C3</f>
+        <v>13.11007268951194</v>
+      </c>
+      <c r="D3">
+        <f>(100/SUM(original_data!$B3:$F3))*original_data!D3</f>
+        <v>12.694704049844235</v>
+      </c>
+      <c r="E3">
+        <f>(100/SUM(original_data!$B3:$F3))*original_data!E3</f>
+        <v>11.915887850467287</v>
+      </c>
+      <c r="F3">
+        <f>(100/SUM(original_data!$B3:$F3))*original_data!F3</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1972</v>
+      </c>
+      <c r="B4">
+        <f>(100/SUM(original_data!$B4:$F4))*original_data!B4</f>
+        <v>12.329822758797844</v>
+      </c>
+      <c r="C4">
+        <f>(100/SUM(original_data!$B4:$F4))*original_data!C4</f>
+        <v>12.817878243000258</v>
+      </c>
+      <c r="D4">
+        <f>(100/SUM(original_data!$B4:$F4))*original_data!D4</f>
+        <v>13.819676342152583</v>
+      </c>
+      <c r="E4">
+        <f>(100/SUM(original_data!$B4:$F4))*original_data!E4</f>
+        <v>11.019779090675573</v>
+      </c>
+      <c r="F4">
+        <f>(100/SUM(original_data!$B4:$F4))*original_data!F4</f>
+        <v>50.01284356537375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1973</v>
+      </c>
+      <c r="B5">
+        <f>(100/SUM(original_data!$B5:$F5))*original_data!B5</f>
+        <v>11.836423672847344</v>
+      </c>
+      <c r="C5">
+        <f>(100/SUM(original_data!$B5:$F5))*original_data!C5</f>
+        <v>12.903225806451612</v>
+      </c>
+      <c r="D5">
+        <f>(100/SUM(original_data!$B5:$F5))*original_data!D5</f>
+        <v>13.335026670053338</v>
+      </c>
+      <c r="E5">
+        <f>(100/SUM(original_data!$B5:$F5))*original_data!E5</f>
+        <v>11.91262382524765</v>
+      </c>
+      <c r="F5">
+        <f>(100/SUM(original_data!$B5:$F5))*original_data!F5</f>
+        <v>50.012700025400051</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1974</v>
+      </c>
+      <c r="B6">
+        <f>(100/SUM(original_data!$B6:$F6))*original_data!B6</f>
+        <v>11.379050489826678</v>
+      </c>
+      <c r="C6">
+        <f>(100/SUM(original_data!$B6:$F6))*original_data!C6</f>
+        <v>12.308465209746297</v>
+      </c>
+      <c r="D6">
+        <f>(100/SUM(original_data!$B6:$F6))*original_data!D6</f>
+        <v>12.358703843255464</v>
+      </c>
+      <c r="E6">
+        <f>(100/SUM(original_data!$B6:$F6))*original_data!E6</f>
+        <v>13.966340115548856</v>
+      </c>
+      <c r="F6">
+        <f>(100/SUM(original_data!$B6:$F6))*original_data!F6</f>
+        <v>49.987440341622701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1975</v>
+      </c>
+      <c r="B7">
+        <f>(100/SUM(original_data!$B7:$F7))*original_data!B7</f>
+        <v>11.602484472049689</v>
+      </c>
+      <c r="C7">
+        <f>(100/SUM(original_data!$B7:$F7))*original_data!C7</f>
+        <v>12.39751552795031</v>
+      </c>
+      <c r="D7">
+        <f>(100/SUM(original_data!$B7:$F7))*original_data!D7</f>
+        <v>11.726708074534161</v>
+      </c>
+      <c r="E7">
+        <f>(100/SUM(original_data!$B7:$F7))*original_data!E7</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="F7">
+        <f>(100/SUM(original_data!$B7:$F7))*original_data!F7</f>
+        <v>49.987577639751549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1976</v>
+      </c>
+      <c r="B8">
+        <f>(100/SUM(original_data!$B8:$F8))*original_data!B8</f>
+        <v>21.790457452041316</v>
+      </c>
+      <c r="C8">
+        <f>(100/SUM(original_data!$B8:$F8))*original_data!C8</f>
+        <v>24.840137727496309</v>
+      </c>
+      <c r="D8">
+        <f>(100/SUM(original_data!$B8:$F8))*original_data!D8</f>
+        <v>23.757993113625187</v>
+      </c>
+      <c r="E8">
+        <f>(100/SUM(original_data!$B8:$F8))*original_data!E8</f>
+        <v>27.988194786030501</v>
+      </c>
+      <c r="F8">
+        <f>(100/SUM(original_data!$B8:$F8))*original_data!F8</f>
+        <v>1.6232169208066898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1977</v>
+      </c>
+      <c r="B9">
+        <f>(100/SUM(original_data!$B9:$F9))*original_data!B9</f>
+        <v>20.778588807785887</v>
+      </c>
+      <c r="C9">
+        <f>(100/SUM(original_data!$B9:$F9))*original_data!C9</f>
+        <v>24.282238442822386</v>
+      </c>
+      <c r="D9">
+        <f>(100/SUM(original_data!$B9:$F9))*original_data!D9</f>
+        <v>23.260340632603409</v>
+      </c>
+      <c r="E9">
+        <f>(100/SUM(original_data!$B9:$F9))*original_data!E9</f>
+        <v>28.467153284671532</v>
+      </c>
+      <c r="F9">
+        <f>(100/SUM(original_data!$B9:$F9))*original_data!F9</f>
+        <v>3.2116788321167888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1978</v>
+      </c>
+      <c r="B10">
+        <f>(100/SUM(original_data!$B10:$F10))*original_data!B10</f>
+        <v>23.603082851637769</v>
+      </c>
+      <c r="C10">
+        <f>(100/SUM(original_data!$B10:$F10))*original_data!C10</f>
+        <v>21.24277456647399</v>
+      </c>
+      <c r="D10">
+        <f>(100/SUM(original_data!$B10:$F10))*original_data!D10</f>
+        <v>24.51830443159923</v>
+      </c>
+      <c r="E10">
+        <f>(100/SUM(original_data!$B10:$F10))*original_data!E10</f>
+        <v>26.49325626204239</v>
+      </c>
+      <c r="F10">
+        <f>(100/SUM(original_data!$B10:$F10))*original_data!F10</f>
+        <v>4.1425818882466281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1979</v>
+      </c>
+      <c r="B11">
+        <f>(100/SUM(original_data!$B11:$F11))*original_data!B11</f>
+        <v>24.511206485455414</v>
+      </c>
+      <c r="C11">
+        <f>(100/SUM(original_data!$B11:$F11))*original_data!C11</f>
+        <v>21.936099189318075</v>
+      </c>
+      <c r="D11">
+        <f>(100/SUM(original_data!$B11:$F11))*original_data!D11</f>
+        <v>20.886981402002863</v>
+      </c>
+      <c r="E11">
+        <f>(100/SUM(original_data!$B11:$F11))*original_data!E11</f>
+        <v>27.086313781592754</v>
+      </c>
+      <c r="F11">
+        <f>(100/SUM(original_data!$B11:$F11))*original_data!F11</f>
+        <v>5.5793991416309021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1980</v>
+      </c>
+      <c r="B12">
+        <f>(100/SUM(original_data!$B12:$F12))*original_data!B12</f>
+        <v>25.542965061378663</v>
+      </c>
+      <c r="C12">
+        <f>(100/SUM(original_data!$B12:$F12))*original_data!C12</f>
+        <v>22.143531633616622</v>
+      </c>
+      <c r="D12">
+        <f>(100/SUM(original_data!$B12:$F12))*original_data!D12</f>
+        <v>20.679886685552411</v>
+      </c>
+      <c r="E12">
+        <f>(100/SUM(original_data!$B12:$F12))*original_data!E12</f>
+        <v>26.534466477809257</v>
+      </c>
+      <c r="F12">
+        <f>(100/SUM(original_data!$B12:$F12))*original_data!F12</f>
+        <v>5.0991501416430607</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1981</v>
+      </c>
+      <c r="B13">
+        <f>(100/SUM(original_data!$B13:$F13))*original_data!B13</f>
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <f>(100/SUM(original_data!$B13:$F13))*original_data!C13</f>
+        <v>21.588785046728972</v>
+      </c>
+      <c r="D13">
+        <f>(100/SUM(original_data!$B13:$F13))*original_data!D13</f>
+        <v>19.813084112149536</v>
+      </c>
+      <c r="E13">
+        <f>(100/SUM(original_data!$B13:$F13))*original_data!E13</f>
+        <v>26.588785046728976</v>
+      </c>
+      <c r="F13">
+        <f>(100/SUM(original_data!$B13:$F13))*original_data!F13</f>
+        <v>7.009345794392523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1982</v>
+      </c>
+      <c r="B14">
+        <f>(100/SUM(original_data!$B14:$F14))*original_data!B14</f>
+        <v>24.884366327474559</v>
+      </c>
+      <c r="C14">
+        <f>(100/SUM(original_data!$B14:$F14))*original_data!C14</f>
+        <v>21.415356151711379</v>
+      </c>
+      <c r="D14">
+        <f>(100/SUM(original_data!$B14:$F14))*original_data!D14</f>
+        <v>19.611470860314526</v>
+      </c>
+      <c r="E14">
+        <f>(100/SUM(original_data!$B14:$F14))*original_data!E14</f>
+        <v>25.485661424606846</v>
+      </c>
+      <c r="F14">
+        <f>(100/SUM(original_data!$B14:$F14))*original_data!F14</f>
+        <v>8.6031452358926934</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1983</v>
+      </c>
+      <c r="B15">
+        <f>(100/SUM(original_data!$B15:$F15))*original_data!B15</f>
+        <v>24.175824175824175</v>
+      </c>
+      <c r="C15">
+        <f>(100/SUM(original_data!$B15:$F15))*original_data!C15</f>
+        <v>21.108058608058609</v>
+      </c>
+      <c r="D15">
+        <f>(100/SUM(original_data!$B15:$F15))*original_data!D15</f>
+        <v>19.505494505494504</v>
+      </c>
+      <c r="E15">
+        <f>(100/SUM(original_data!$B15:$F15))*original_data!E15</f>
+        <v>25.686813186813186</v>
+      </c>
+      <c r="F15">
+        <f>(100/SUM(original_data!$B15:$F15))*original_data!F15</f>
+        <v>9.5238095238095237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1984</v>
+      </c>
+      <c r="B16">
+        <f>(100/SUM(original_data!$B16:$F16))*original_data!B16</f>
+        <v>23.49206349206349</v>
+      </c>
+      <c r="C16">
+        <f>(100/SUM(original_data!$B16:$F16))*original_data!C16</f>
+        <v>20.997732426303855</v>
+      </c>
+      <c r="D16">
+        <f>(100/SUM(original_data!$B16:$F16))*original_data!D16</f>
+        <v>19.41043083900227</v>
+      </c>
+      <c r="E16">
+        <f>(100/SUM(original_data!$B16:$F16))*original_data!E16</f>
+        <v>25.351473922902493</v>
+      </c>
+      <c r="F16">
+        <f>(100/SUM(original_data!$B16:$F16))*original_data!F16</f>
+        <v>10.748299319727892</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1985</v>
+      </c>
+      <c r="B17">
+        <f>(100/SUM(original_data!$B17:$F17))*original_data!B17</f>
+        <v>23.090745732255165</v>
+      </c>
+      <c r="C17">
+        <f>(100/SUM(original_data!$B17:$F17))*original_data!C17</f>
+        <v>20.754716981132077</v>
+      </c>
+      <c r="D17">
+        <f>(100/SUM(original_data!$B17:$F17))*original_data!D17</f>
+        <v>19.182389937106915</v>
+      </c>
+      <c r="E17">
+        <f>(100/SUM(original_data!$B17:$F17))*original_data!E17</f>
+        <v>25.247079964061097</v>
+      </c>
+      <c r="F17">
+        <f>(100/SUM(original_data!$B17:$F17))*original_data!F17</f>
+        <v>11.725067385444744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1986</v>
+      </c>
+      <c r="B18">
+        <f>(100/SUM(original_data!$B18:$F18))*original_data!B18</f>
+        <v>22.19750889679716</v>
+      </c>
+      <c r="C18">
+        <f>(100/SUM(original_data!$B18:$F18))*original_data!C18</f>
+        <v>20.818505338078296</v>
+      </c>
+      <c r="D18">
+        <f>(100/SUM(original_data!$B18:$F18))*original_data!D18</f>
+        <v>19.217081850533813</v>
+      </c>
+      <c r="E18">
+        <f>(100/SUM(original_data!$B18:$F18))*original_data!E18</f>
+        <v>25.489323843416379</v>
+      </c>
+      <c r="F18">
+        <f>(100/SUM(original_data!$B18:$F18))*original_data!F18</f>
+        <v>12.277580071174379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1987</v>
+      </c>
+      <c r="B19">
+        <f>(100/SUM(original_data!$B19:$F19))*original_data!B19</f>
+        <v>21.507271925958573</v>
+      </c>
+      <c r="C19">
+        <f>(100/SUM(original_data!$B19:$F19))*original_data!C19</f>
+        <v>20.802115469369767</v>
+      </c>
+      <c r="D19">
+        <f>(100/SUM(original_data!$B19:$F19))*original_data!D19</f>
+        <v>19.171441163508153</v>
+      </c>
+      <c r="E19">
+        <f>(100/SUM(original_data!$B19:$F19))*original_data!E19</f>
+        <v>24.8126928162186</v>
+      </c>
+      <c r="F19">
+        <f>(100/SUM(original_data!$B19:$F19))*original_data!F19</f>
+        <v>13.706478624944911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1988</v>
+      </c>
+      <c r="B20">
+        <f>(100/SUM(original_data!$B20:$F20))*original_data!B20</f>
+        <v>20.515058926233085</v>
+      </c>
+      <c r="C20">
+        <f>(100/SUM(original_data!$B20:$F20))*original_data!C20</f>
+        <v>20.68965517241379</v>
+      </c>
+      <c r="D20">
+        <f>(100/SUM(original_data!$B20:$F20))*original_data!D20</f>
+        <v>19.20558707987778</v>
+      </c>
+      <c r="E20">
+        <f>(100/SUM(original_data!$B20:$F20))*original_data!E20</f>
+        <v>24.792666957660405</v>
+      </c>
+      <c r="F20">
+        <f>(100/SUM(original_data!$B20:$F20))*original_data!F20</f>
+        <v>14.797031863814926</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1989</v>
+      </c>
+      <c r="B21">
+        <f>(100/SUM(original_data!$B21:$F21))*original_data!B21</f>
+        <v>20.501730103806231</v>
+      </c>
+      <c r="C21">
+        <f>(100/SUM(original_data!$B21:$F21))*original_data!C21</f>
+        <v>20.588235294117645</v>
+      </c>
+      <c r="D21">
+        <f>(100/SUM(original_data!$B21:$F21))*original_data!D21</f>
+        <v>19.20415224913495</v>
+      </c>
+      <c r="E21">
+        <f>(100/SUM(original_data!$B21:$F21))*original_data!E21</f>
+        <v>24.091695501730104</v>
+      </c>
+      <c r="F21">
+        <f>(100/SUM(original_data!$B21:$F21))*original_data!F21</f>
+        <v>15.614186851211073</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1990</v>
+      </c>
+      <c r="B22">
+        <f>(100/SUM(original_data!$B22:$F22))*original_data!B22</f>
+        <v>20.488641234462065</v>
+      </c>
+      <c r="C22">
+        <f>(100/SUM(original_data!$B22:$F22))*original_data!C22</f>
+        <v>20.188598371195884</v>
+      </c>
+      <c r="D22">
+        <f>(100/SUM(original_data!$B22:$F22))*original_data!D22</f>
+        <v>19.245606515216458</v>
+      </c>
+      <c r="E22">
+        <f>(100/SUM(original_data!$B22:$F22))*original_data!E22</f>
+        <v>23.917702528932701</v>
+      </c>
+      <c r="F22">
+        <f>(100/SUM(original_data!$B22:$F22))*original_data!F22</f>
+        <v>16.159451350192882</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1991</v>
+      </c>
+      <c r="B23">
+        <f>(100/SUM(original_data!$B23:$F23))*original_data!B23</f>
+        <v>20.399490012749681</v>
+      </c>
+      <c r="C23">
+        <f>(100/SUM(original_data!$B23:$F23))*original_data!C23</f>
+        <v>20.101997450063752</v>
+      </c>
+      <c r="D23">
+        <f>(100/SUM(original_data!$B23:$F23))*original_data!D23</f>
+        <v>18.997025074373141</v>
+      </c>
+      <c r="E23">
+        <f>(100/SUM(original_data!$B23:$F23))*original_data!E23</f>
+        <v>23.501912452188698</v>
+      </c>
+      <c r="F23">
+        <f>(100/SUM(original_data!$B23:$F23))*original_data!F23</f>
+        <v>16.999575010624735</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1992</v>
+      </c>
+      <c r="B24">
+        <f>(100/SUM(original_data!$B24:$F24))*original_data!B24</f>
+        <v>20.117845117845118</v>
+      </c>
+      <c r="C24">
+        <f>(100/SUM(original_data!$B24:$F24))*original_data!C24</f>
+        <v>19.907407407407408</v>
+      </c>
+      <c r="D24">
+        <f>(100/SUM(original_data!$B24:$F24))*original_data!D24</f>
+        <v>18.897306397306398</v>
+      </c>
+      <c r="E24">
+        <f>(100/SUM(original_data!$B24:$F24))*original_data!E24</f>
+        <v>23.400673400673398</v>
+      </c>
+      <c r="F24">
+        <f>(100/SUM(original_data!$B24:$F24))*original_data!F24</f>
+        <v>17.676767676767675</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1993</v>
+      </c>
+      <c r="B25">
+        <f>(100/SUM(original_data!$B25:$F25))*original_data!B25</f>
+        <v>20.083507306889352</v>
+      </c>
+      <c r="C25">
+        <f>(100/SUM(original_data!$B25:$F25))*original_data!C25</f>
+        <v>19.916492693110648</v>
+      </c>
+      <c r="D25">
+        <f>(100/SUM(original_data!$B25:$F25))*original_data!D25</f>
+        <v>18.914405010438415</v>
+      </c>
+      <c r="E25">
+        <f>(100/SUM(original_data!$B25:$F25))*original_data!E25</f>
+        <v>22.881002087682678</v>
+      </c>
+      <c r="F25">
+        <f>(100/SUM(original_data!$B25:$F25))*original_data!F25</f>
+        <v>18.204592901878918</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1994</v>
+      </c>
+      <c r="B26">
+        <f>(100/SUM(original_data!$B26:$F26))*original_data!B26</f>
+        <v>19.900497512437813</v>
+      </c>
+      <c r="C26">
+        <f>(100/SUM(original_data!$B26:$F26))*original_data!C26</f>
+        <v>19.69320066334992</v>
+      </c>
+      <c r="D26">
+        <f>(100/SUM(original_data!$B26:$F26))*original_data!D26</f>
+        <v>18.698175787728026</v>
+      </c>
+      <c r="E26">
+        <f>(100/SUM(original_data!$B26:$F26))*original_data!E26</f>
+        <v>22.719734660033172</v>
+      </c>
+      <c r="F26">
+        <f>(100/SUM(original_data!$B26:$F26))*original_data!F26</f>
+        <v>18.98839137645108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1995</v>
+      </c>
+      <c r="B27">
+        <f>(100/SUM(original_data!$B27:$F27))*original_data!B27</f>
+        <v>19.884963023829087</v>
+      </c>
+      <c r="C27">
+        <f>(100/SUM(original_data!$B27:$F27))*original_data!C27</f>
+        <v>19.72062448644207</v>
+      </c>
+      <c r="D27">
+        <f>(100/SUM(original_data!$B27:$F27))*original_data!D27</f>
+        <v>18.693508627773213</v>
+      </c>
+      <c r="E27">
+        <f>(100/SUM(original_data!$B27:$F27))*original_data!E27</f>
+        <v>22.514379622021366</v>
+      </c>
+      <c r="F27">
+        <f>(100/SUM(original_data!$B27:$F27))*original_data!F27</f>
+        <v>19.186524239934265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1996</v>
+      </c>
+      <c r="B28">
+        <f>(100/SUM(original_data!$B28:$F28))*original_data!B28</f>
+        <v>19.771708112515288</v>
+      </c>
+      <c r="C28">
+        <f>(100/SUM(original_data!$B28:$F28))*original_data!C28</f>
+        <v>19.690175295556465</v>
+      </c>
+      <c r="D28">
+        <f>(100/SUM(original_data!$B28:$F28))*original_data!D28</f>
+        <v>18.711781492050552</v>
+      </c>
+      <c r="E28">
+        <f>(100/SUM(original_data!$B28:$F28))*original_data!E28</f>
+        <v>22.217692621280069</v>
+      </c>
+      <c r="F28">
+        <f>(100/SUM(original_data!$B28:$F28))*original_data!F28</f>
+        <v>19.608642478597638</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1997</v>
+      </c>
+      <c r="B29">
+        <f>(100/SUM(original_data!$B29:$F29))*original_data!B29</f>
+        <v>19.587211655200321</v>
+      </c>
+      <c r="C29">
+        <f>(100/SUM(original_data!$B29:$F29))*original_data!C29</f>
+        <v>19.506272764063134</v>
+      </c>
+      <c r="D29">
+        <f>(100/SUM(original_data!$B29:$F29))*original_data!D29</f>
+        <v>18.494536624848241</v>
+      </c>
+      <c r="E29">
+        <f>(100/SUM(original_data!$B29:$F29))*original_data!E29</f>
+        <v>22.015378389316066</v>
+      </c>
+      <c r="F29">
+        <f>(100/SUM(original_data!$B29:$F29))*original_data!F29</f>
+        <v>20.396600566572236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1998</v>
+      </c>
+      <c r="B30">
+        <f>(100/SUM(original_data!$B30:$F30))*original_data!B30</f>
+        <v>19.51023685266961</v>
+      </c>
+      <c r="C30">
+        <f>(100/SUM(original_data!$B30:$F30))*original_data!C30</f>
+        <v>19.389803291850662</v>
+      </c>
+      <c r="D30">
+        <f>(100/SUM(original_data!$B30:$F30))*original_data!D30</f>
+        <v>18.386190285026093</v>
+      </c>
+      <c r="E30">
+        <f>(100/SUM(original_data!$B30:$F30))*original_data!E30</f>
+        <v>21.798474508229624</v>
+      </c>
+      <c r="F30">
+        <f>(100/SUM(original_data!$B30:$F30))*original_data!F30</f>
+        <v>20.915295062224004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1999</v>
+      </c>
+      <c r="B31">
+        <f>(100/SUM(original_data!$B31:$F31))*original_data!B31</f>
+        <v>19.402390438247011</v>
+      </c>
+      <c r="C31">
+        <f>(100/SUM(original_data!$B31:$F31))*original_data!C31</f>
+        <v>19.203187250996017</v>
+      </c>
+      <c r="D31">
+        <f>(100/SUM(original_data!$B31:$F31))*original_data!D31</f>
+        <v>18.28685258964143</v>
+      </c>
+      <c r="E31">
+        <f>(100/SUM(original_data!$B31:$F31))*original_data!E31</f>
+        <v>21.713147410358562</v>
+      </c>
+      <c r="F31">
+        <f>(100/SUM(original_data!$B31:$F31))*original_data!F31</f>
+        <v>21.394422310756969</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2000</v>
+      </c>
+      <c r="B32">
+        <f>(100/SUM(original_data!$B32:$F32))*original_data!B32</f>
+        <v>19.382911392405063</v>
+      </c>
+      <c r="C32">
+        <f>(100/SUM(original_data!$B32:$F32))*original_data!C32</f>
+        <v>19.224683544303797</v>
+      </c>
+      <c r="D32">
+        <f>(100/SUM(original_data!$B32:$F32))*original_data!D32</f>
+        <v>18.196202531645568</v>
+      </c>
+      <c r="E32">
+        <f>(100/SUM(original_data!$B32:$F32))*original_data!E32</f>
+        <v>21.598101265822784</v>
+      </c>
+      <c r="F32">
+        <f>(100/SUM(original_data!$B32:$F32))*original_data!F32</f>
+        <v>21.598101265822784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B33">
+        <f>(100/SUM(original_data!$B33:$F33))*original_data!B33</f>
+        <v>19.277581468394189</v>
+      </c>
+      <c r="C33">
+        <f>(100/SUM(original_data!$B33:$F33))*original_data!C33</f>
+        <v>19.002748331370238</v>
+      </c>
+      <c r="D33">
+        <f>(100/SUM(original_data!$B33:$F33))*original_data!D33</f>
+        <v>18.217510797016097</v>
+      </c>
+      <c r="E33">
+        <f>(100/SUM(original_data!$B33:$F33))*original_data!E33</f>
+        <v>21.515508441303496</v>
+      </c>
+      <c r="F33">
+        <f>(100/SUM(original_data!$B33:$F33))*original_data!F33</f>
+        <v>21.986650961915977</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B34">
+        <f>(100/SUM(original_data!$B34:$F34))*original_data!B34</f>
+        <v>19.281811085089775</v>
+      </c>
+      <c r="C34">
+        <f>(100/SUM(original_data!$B34:$F34))*original_data!C34</f>
+        <v>19.008587041373925</v>
+      </c>
+      <c r="D34">
+        <f>(100/SUM(original_data!$B34:$F34))*original_data!D34</f>
+        <v>18.227946916471506</v>
+      </c>
+      <c r="E34">
+        <f>(100/SUM(original_data!$B34:$F34))*original_data!E34</f>
+        <v>21.506635441061668</v>
+      </c>
+      <c r="F34">
+        <f>(100/SUM(original_data!$B34:$F34))*original_data!F34</f>
+        <v>21.975019516003123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B35">
+        <f>(100/SUM(original_data!$B35:$F35))*original_data!B35</f>
+        <v>20.620155038759691</v>
+      </c>
+      <c r="C35">
+        <f>(100/SUM(original_data!$B35:$F35))*original_data!C35</f>
+        <v>18.720930232558143</v>
+      </c>
+      <c r="D35">
+        <f>(100/SUM(original_data!$B35:$F35))*original_data!D35</f>
+        <v>20.736434108527131</v>
+      </c>
+      <c r="E35">
+        <f>(100/SUM(original_data!$B35:$F35))*original_data!E35</f>
+        <v>15.387596899224809</v>
+      </c>
+      <c r="F35">
+        <f>(100/SUM(original_data!$B35:$F35))*original_data!F35</f>
+        <v>24.534883720930235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B36">
+        <f>(100/SUM(original_data!$B36:$F36))*original_data!B36</f>
+        <v>20.82371054657429</v>
+      </c>
+      <c r="C36">
+        <f>(100/SUM(original_data!$B36:$F36))*original_data!C36</f>
+        <v>17.975365665896845</v>
+      </c>
+      <c r="D36">
+        <f>(100/SUM(original_data!$B36:$F36))*original_data!D36</f>
+        <v>20.939183987682839</v>
+      </c>
+      <c r="E36">
+        <f>(100/SUM(original_data!$B36:$F36))*original_data!E36</f>
+        <v>15.280985373364128</v>
+      </c>
+      <c r="F36">
+        <f>(100/SUM(original_data!$B36:$F36))*original_data!F36</f>
+        <v>24.980754426481912</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B37">
+        <f>(100/SUM(original_data!$B37:$F37))*original_data!B37</f>
+        <v>21.496754486445202</v>
+      </c>
+      <c r="C37">
+        <f>(100/SUM(original_data!$B37:$F37))*original_data!C37</f>
+        <v>17.487590683466969</v>
+      </c>
+      <c r="D37">
+        <f>(100/SUM(original_data!$B37:$F37))*original_data!D37</f>
+        <v>19.740358915616643</v>
+      </c>
+      <c r="E37">
+        <f>(100/SUM(original_data!$B37:$F37))*original_data!E37</f>
+        <v>15.540282550591826</v>
+      </c>
+      <c r="F37">
+        <f>(100/SUM(original_data!$B37:$F37))*original_data!F37</f>
+        <v>25.735013363879339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B38">
+        <f>(100/SUM(original_data!$B38:$F38))*original_data!B38</f>
+        <v>21.385314155942467</v>
+      </c>
+      <c r="C38">
+        <f>(100/SUM(original_data!$B38:$F38))*original_data!C38</f>
+        <v>18.205904617713848</v>
+      </c>
+      <c r="D38">
+        <f>(100/SUM(original_data!$B38:$F38))*original_data!D38</f>
+        <v>19.984859954579864</v>
+      </c>
+      <c r="E38">
+        <f>(100/SUM(original_data!$B38:$F38))*original_data!E38</f>
+        <v>15.140045420136259</v>
+      </c>
+      <c r="F38">
+        <f>(100/SUM(original_data!$B38:$F38))*original_data!F38</f>
+        <v>25.283875851627553</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B39">
+        <f>(100/SUM(original_data!$B39:$F39))*original_data!B39</f>
+        <v>21.058558558558559</v>
+      </c>
+      <c r="C39">
+        <f>(100/SUM(original_data!$B39:$F39))*original_data!C39</f>
+        <v>17.454954954954957</v>
+      </c>
+      <c r="D39">
+        <f>(100/SUM(original_data!$B39:$F39))*original_data!D39</f>
+        <v>19.707207207207208</v>
+      </c>
+      <c r="E39">
+        <f>(100/SUM(original_data!$B39:$F39))*original_data!E39</f>
+        <v>14.902402402402403</v>
+      </c>
+      <c r="F39">
+        <f>(100/SUM(original_data!$B39:$F39))*original_data!F39</f>
+        <v>26.876876876876878</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B40">
+        <f>(100/SUM(original_data!$B40:$F40))*original_data!B40</f>
+        <v>21.39673105497771</v>
+      </c>
+      <c r="C40">
+        <f>(100/SUM(original_data!$B40:$F40))*original_data!C40</f>
+        <v>35.995542347696876</v>
+      </c>
+      <c r="D40">
+        <f>(100/SUM(original_data!$B40:$F40))*original_data!D40</f>
+        <v>30.423476968796429</v>
+      </c>
+      <c r="E40">
+        <f>(100/SUM(original_data!$B40:$F40))*original_data!E40</f>
+        <v>9.3610698365527476</v>
+      </c>
+      <c r="F40">
+        <f>(100/SUM(original_data!$B40:$F40))*original_data!F40</f>
+        <v>2.8231797919762256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B41">
+        <f>(100/SUM(original_data!$B41:$F41))*original_data!B41</f>
+        <v>21.468092954629288</v>
+      </c>
+      <c r="C41">
+        <f>(100/SUM(original_data!$B41:$F41))*original_data!C41</f>
+        <v>36.665437108078201</v>
+      </c>
+      <c r="D41">
+        <f>(100/SUM(original_data!$B41:$F41))*original_data!D41</f>
+        <v>29.620066396163775</v>
+      </c>
+      <c r="E41">
+        <f>(100/SUM(original_data!$B41:$F41))*original_data!E41</f>
+        <v>8.0413131685724828</v>
+      </c>
+      <c r="F41">
+        <f>(100/SUM(original_data!$B41:$F41))*original_data!F41</f>
+        <v>4.2050903725562518</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B42">
+        <f>(100/SUM(original_data!$B42:$F42))*original_data!B42</f>
+        <v>21.72957127152803</v>
+      </c>
+      <c r="C42">
+        <f>(100/SUM(original_data!$B42:$F42))*original_data!C42</f>
+        <v>36.386954928545251</v>
+      </c>
+      <c r="D42">
+        <f>(100/SUM(original_data!$B42:$F42))*original_data!D42</f>
+        <v>28.948332722609017</v>
+      </c>
+      <c r="E42">
+        <f>(100/SUM(original_data!$B42:$F42))*original_data!E42</f>
+        <v>7.9149871747893004</v>
+      </c>
+      <c r="F42">
+        <f>(100/SUM(original_data!$B42:$F42))*original_data!F42</f>
+        <v>5.0201539025283992</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B43">
+        <f>(100/SUM(original_data!$B43:$F43))*original_data!B43</f>
+        <v>20.824215900802333</v>
+      </c>
+      <c r="C43">
+        <f>(100/SUM(original_data!$B43:$F43))*original_data!C43</f>
+        <v>36.323851203501093</v>
+      </c>
+      <c r="D43">
+        <f>(100/SUM(original_data!$B43:$F43))*original_data!D43</f>
+        <v>29.431072210065643</v>
+      </c>
+      <c r="E43">
+        <f>(100/SUM(original_data!$B43:$F43))*original_data!E43</f>
+        <v>8.0233406272793584</v>
+      </c>
+      <c r="F43">
+        <f>(100/SUM(original_data!$B43:$F43))*original_data!F43</f>
+        <v>5.3975200583515681</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F43" sqref="A1:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,30 +1703,31 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1918</v>
+      </c>
+      <c r="C1">
+        <f>(1918+1938)/2</f>
+        <v>1928</v>
+      </c>
+      <c r="D1">
+        <f>(1939+1959)/2</f>
+        <v>1949</v>
+      </c>
+      <c r="E1">
+        <f>ROUND((1960+1975)/2,0)</f>
+        <v>1968</v>
+      </c>
+      <c r="F1">
+        <f>ROUND((1976+2015)/2,2)</f>
+        <v>1995.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -678,7 +1747,7 @@
         <v>19.04</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -698,7 +1767,7 @@
         <v>19.260000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -718,7 +1787,7 @@
         <v>19.47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -738,7 +1807,7 @@
         <v>19.690000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -758,7 +1827,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -778,7 +1847,7 @@
         <v>20.12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -797,11 +1866,8 @@
       <c r="F8">
         <v>0.33</v>
       </c>
-      <c r="G8">
-        <v>20.329999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -820,11 +1886,8 @@
       <c r="F9">
         <v>0.66</v>
       </c>
-      <c r="G9">
-        <v>20.55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -843,11 +1906,8 @@
       <c r="F10">
         <v>0.86</v>
       </c>
-      <c r="G10">
-        <v>20.76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -866,11 +1926,8 @@
       <c r="F11">
         <v>1.17</v>
       </c>
-      <c r="G11">
-        <v>20.98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -889,11 +1946,8 @@
       <c r="F12">
         <v>1.08</v>
       </c>
-      <c r="G12">
-        <v>21.19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -912,11 +1966,8 @@
       <c r="F13">
         <v>1.5</v>
       </c>
-      <c r="G13">
-        <v>21.41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -935,11 +1986,8 @@
       <c r="F14">
         <v>1.86</v>
       </c>
-      <c r="G14">
-        <v>21.62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -958,11 +2006,8 @@
       <c r="F15">
         <v>2.08</v>
       </c>
-      <c r="G15">
-        <v>21.83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -981,11 +2026,8 @@
       <c r="F16">
         <v>2.37</v>
       </c>
-      <c r="G16">
-        <v>22.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1004,11 +2046,8 @@
       <c r="F17">
         <v>2.61</v>
       </c>
-      <c r="G17">
-        <v>22.26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1027,11 +2066,8 @@
       <c r="F18">
         <v>2.76</v>
       </c>
-      <c r="G18">
-        <v>22.48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1050,11 +2086,8 @@
       <c r="F19">
         <v>3.11</v>
       </c>
-      <c r="G19">
-        <v>22.69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -1073,11 +2106,8 @@
       <c r="F20">
         <v>3.39</v>
       </c>
-      <c r="G20">
-        <v>22.91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -1096,11 +2126,8 @@
       <c r="F21">
         <v>3.61</v>
       </c>
-      <c r="G21">
-        <v>23.12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -1119,11 +2146,8 @@
       <c r="F22">
         <v>3.77</v>
       </c>
-      <c r="G22">
-        <v>23.34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -1142,11 +2166,8 @@
       <c r="F23">
         <v>4</v>
       </c>
-      <c r="G23">
-        <v>23.55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -1165,11 +2186,8 @@
       <c r="F24">
         <v>4.2</v>
       </c>
-      <c r="G24">
-        <v>23.76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -1188,11 +2206,8 @@
       <c r="F25">
         <v>4.3600000000000003</v>
       </c>
-      <c r="G25">
-        <v>23.95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -1211,14 +2226,8 @@
       <c r="F26">
         <v>4.58</v>
       </c>
-      <c r="G26">
-        <v>24.14</v>
-      </c>
-      <c r="I26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -1237,11 +2246,8 @@
       <c r="F27">
         <v>4.67</v>
       </c>
-      <c r="G27">
-        <v>24.34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -1260,11 +2266,8 @@
       <c r="F28">
         <v>4.8099999999999996</v>
       </c>
-      <c r="G28">
-        <v>24.53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -1283,11 +2286,8 @@
       <c r="F29">
         <v>5.04</v>
       </c>
-      <c r="G29">
-        <v>24.72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -1306,11 +2306,8 @@
       <c r="F30">
         <v>5.21</v>
       </c>
-      <c r="G30">
-        <v>24.91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -1329,11 +2326,8 @@
       <c r="F31">
         <v>5.37</v>
       </c>
-      <c r="G31">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -1352,78 +2346,69 @@
       <c r="F32">
         <v>5.46</v>
       </c>
-      <c r="G32">
-        <v>25.28</v>
-      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>2001</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>4.91</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>4.84</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>4.6399999999999997</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>5.48</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>5.6</v>
       </c>
-      <c r="G33">
-        <v>25.47</v>
-      </c>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>2002</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>4.9400000000000004</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>4.87</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>4.67</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>5.51</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>5.63</v>
       </c>
-      <c r="G34">
-        <v>25.62</v>
-      </c>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>2003</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>5.32</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>4.83</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>5.35</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>3.97</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>6.33</v>
       </c>
-      <c r="G35">
-        <v>25.8</v>
-      </c>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1444,9 +2429,7 @@
       <c r="F36" s="1">
         <v>6.49</v>
       </c>
-      <c r="G36" s="1">
-        <v>25.99</v>
-      </c>
+      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1467,9 +2450,7 @@
       <c r="F37" s="1">
         <v>6.74</v>
       </c>
-      <c r="G37" s="1">
-        <v>26.2</v>
-      </c>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1490,9 +2471,7 @@
       <c r="F38" s="1">
         <v>6.68</v>
       </c>
-      <c r="G38" s="1">
-        <v>26.42</v>
-      </c>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -1513,28 +2492,26 @@
       <c r="F39" s="1">
         <v>7.16</v>
       </c>
-      <c r="G39" s="1">
-        <v>26.66</v>
-      </c>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B40" s="1">
         <v>5.76</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>9.69</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>8.19</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>2.52</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>0.76</v>
-      </c>
-      <c r="F40" s="1">
-        <v>26.91</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -1557,9 +2534,7 @@
       <c r="F41" s="1">
         <v>1.1399999999999999</v>
       </c>
-      <c r="G41" s="1">
-        <v>27.11</v>
-      </c>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -1580,9 +2555,7 @@
       <c r="F42" s="1">
         <v>1.37</v>
       </c>
-      <c r="G42" s="1">
-        <v>27.27</v>
-      </c>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -1603,26 +2576,12 @@
       <c r="F43" s="1">
         <v>1.48</v>
       </c>
-      <c r="G43" s="1">
-        <v>27.42</v>
-      </c>
+      <c r="G43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working on housing stock
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/energy_fact_file_housing_stock_age.xlsx
+++ b/data/residential_model/_EXCELFILES/energy_fact_file_housing_stock_age.xlsx
@@ -34,7 +34,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,6 +44,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -60,9 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -77,7 +84,3123 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data_prepared!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data_prepared!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>25.459317585301839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.558670820353061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.66598150051388</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.678861788617887</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.752385735811149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.199205166418285</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.790457452041316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.778588807785887</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.603082851637769</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.511206485455414</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.542965061378663</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.884366327474559</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.175824175824175</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.49206349206349</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.090745732255165</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.19750889679716</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.507271925958573</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.515058926233085</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.501730103806231</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.488641234462065</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.399490012749681</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.117845117845118</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.083507306889352</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.900497512437813</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19.884963023829087</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.771708112515288</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.587211655200321</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19.51023685266961</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.402390438247011</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19.382911392405063</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.277581468394189</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19.281811085089775</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.620155038759691</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.82371054657429</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21.496754486445202</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>21.385314155942467</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>21.058558558558559</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>21.39673105497771</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>21.468092954629288</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>21.72957127152803</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.824215900802333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data_prepared!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data_prepared!$C$2:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>27.191601049868769</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.220145379023879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.642343268242556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.8130081300813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.610748367654445</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.788872329855941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.840137727496309</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.282238442822386</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.24277456647399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.936099189318075</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.143531633616622</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.588785046728972</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.415356151711379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.108058608058609</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.997732426303855</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.754716981132077</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20.818505338078296</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.802115469369767</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.68965517241379</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.588235294117645</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.188598371195884</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.101997450063752</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.907407407407408</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.916492693110648</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.69320066334992</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19.72062448644207</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.690175295556465</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.506272764063134</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19.389803291850662</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.203187250996017</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19.224683544303797</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.002748331370238</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19.008587041373925</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18.720930232558143</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17.975365665896845</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.487590683466969</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18.205904617713848</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17.454954954954957</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>35.995542347696876</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>36.665437108078201</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>36.386954928545251</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>36.323851203501093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data_prepared!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data_prepared!$D$2:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>26.2992125984252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.38940809968847</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.646454265159306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.676829268292682</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.711200401808135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.447590660705416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.757993113625187</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.260340632603409</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.51830443159923</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.886981402002863</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.679886685552411</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.813084112149536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.611470860314526</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.505494505494504</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.41043083900227</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.182389937106915</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.217081850533813</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.171441163508153</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.20558707987778</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.20415224913495</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.245606515216458</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18.997025074373141</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.897306397306398</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18.914405010438415</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.698175787728026</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18.693508627773213</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.711781492050552</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18.494536624848241</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>18.386190285026093</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18.28685258964143</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18.196202531645568</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18.217510797016097</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>18.227946916471506</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.736434108527131</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.939183987682839</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19.740358915616643</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19.984859954579864</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.707207207207208</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30.423476968796429</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>29.620066396163775</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28.948332722609017</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>29.431072210065643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data_prepared!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data_prepared!$E$2:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>21.049868766404202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.831775700934575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.04522096608428</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.831300813008131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.925665494726264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.564331843020369</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.988194786030501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.467153284671532</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.49325626204239</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.086313781592754</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.534466477809257</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.588785046728976</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.485661424606846</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.686813186813186</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.351473922902493</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.247079964061097</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.489323843416379</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.8126928162186</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.792666957660405</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.091695501730104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.917702528932701</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.501912452188698</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.400673400673398</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.881002087682678</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22.719734660033172</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.514379622021366</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22.217692621280069</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22.015378389316066</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21.798474508229624</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.713147410358562</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21.598101265822784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.515508441303496</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>21.506635441061668</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.387596899224809</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.280985373364128</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.540282550591826</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15.140045420136259</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.902402402402403</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.3610698365527476</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.0413131685724828</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.9149871747893004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.0233406272793584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data_prepared!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data_prepared!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6232169208066898</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2116788321167888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1425818882466281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5793991416309021</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0991501416430607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.009345794392523</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.6031452358926934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5238095238095237</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.748299319727892</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.725067385444744</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.277580071174379</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.706478624944911</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.797031863814926</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.614186851211073</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16.159451350192882</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16.999575010624735</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.676767676767675</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18.204592901878918</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.98839137645108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19.186524239934265</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.608642478597638</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20.396600566572236</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20.915295062224004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.394422310756969</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21.598101265822784</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.986650961915977</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>21.975019516003123</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.534883720930235</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24.980754426481912</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>25.735013363879339</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>25.283875851627553</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>26.876876876876878</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.8231797919762256</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.2050903725562518</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.0201539025283992</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.3975200583515681</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="75117696"/>
+        <c:axId val="74997120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="75117696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74997120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74997120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75117696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Number of Housing with respective </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>housing ages over time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>original_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1918</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>original_data!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>original_data!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.91</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.65</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.76</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.82</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>original_data!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1928</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>original_data!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>original_data!$C$2:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.6900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.76</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.7699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.69</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.94</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.93</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.9600000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>original_data!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1949</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>original_data!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>original_data!$D$2:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.47</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.51</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.6399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.35</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.17</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.0299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.07</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>original_data!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1968</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>original_data!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>original_data!$E$2:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.51</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.57</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.58</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.48</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.44</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.48</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.51</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.97</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.97</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.97</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>original_data!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1995.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>original_data!$A$2:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>original_data!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="6">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.77</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.21</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.49</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.74</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.68</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.16</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="72673536"/>
+        <c:axId val="72672000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="72673536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72672000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="72672000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>million</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of houses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72673536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -308,6 +3431,36 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -603,7 +3756,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,23 +3791,23 @@
       </c>
       <c r="B2">
         <f>(100/SUM(original_data!$B2:$F2))*original_data!B2</f>
-        <v>12.733000787608297</v>
+        <v>25.459317585301839</v>
       </c>
       <c r="C2">
         <f>(100/SUM(original_data!$B2:$F2))*original_data!C2</f>
-        <v>13.599369913363088</v>
+        <v>27.191601049868769</v>
       </c>
       <c r="D2">
         <f>(100/SUM(original_data!$B2:$F2))*original_data!D2</f>
-        <v>13.153058545550014</v>
+        <v>26.2992125984252</v>
       </c>
       <c r="E2">
         <f>(100/SUM(original_data!$B2:$F2))*original_data!E2</f>
-        <v>10.527697558414284</v>
+        <v>21.049868766404202</v>
       </c>
       <c r="F2">
         <f>(100/SUM(original_data!$B2:$F2))*original_data!F2</f>
-        <v>49.986873195064327</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,23 +3816,23 @@
       </c>
       <c r="B3">
         <f>(100/SUM(original_data!$B3:$F3))*original_data!B3</f>
-        <v>12.279335410176531</v>
+        <v>24.558670820353061</v>
       </c>
       <c r="C3">
         <f>(100/SUM(original_data!$B3:$F3))*original_data!C3</f>
-        <v>13.11007268951194</v>
+        <v>26.220145379023879</v>
       </c>
       <c r="D3">
         <f>(100/SUM(original_data!$B3:$F3))*original_data!D3</f>
-        <v>12.694704049844235</v>
+        <v>25.38940809968847</v>
       </c>
       <c r="E3">
         <f>(100/SUM(original_data!$B3:$F3))*original_data!E3</f>
-        <v>11.915887850467287</v>
+        <v>23.831775700934575</v>
       </c>
       <c r="F3">
         <f>(100/SUM(original_data!$B3:$F3))*original_data!F3</f>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,23 +3841,23 @@
       </c>
       <c r="B4">
         <f>(100/SUM(original_data!$B4:$F4))*original_data!B4</f>
-        <v>12.329822758797844</v>
+        <v>24.66598150051388</v>
       </c>
       <c r="C4">
         <f>(100/SUM(original_data!$B4:$F4))*original_data!C4</f>
-        <v>12.817878243000258</v>
+        <v>25.642343268242556</v>
       </c>
       <c r="D4">
         <f>(100/SUM(original_data!$B4:$F4))*original_data!D4</f>
-        <v>13.819676342152583</v>
+        <v>27.646454265159306</v>
       </c>
       <c r="E4">
         <f>(100/SUM(original_data!$B4:$F4))*original_data!E4</f>
-        <v>11.019779090675573</v>
+        <v>22.04522096608428</v>
       </c>
       <c r="F4">
         <f>(100/SUM(original_data!$B4:$F4))*original_data!F4</f>
-        <v>50.01284356537375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,23 +3866,23 @@
       </c>
       <c r="B5">
         <f>(100/SUM(original_data!$B5:$F5))*original_data!B5</f>
-        <v>11.836423672847344</v>
+        <v>23.678861788617887</v>
       </c>
       <c r="C5">
         <f>(100/SUM(original_data!$B5:$F5))*original_data!C5</f>
-        <v>12.903225806451612</v>
+        <v>25.8130081300813</v>
       </c>
       <c r="D5">
         <f>(100/SUM(original_data!$B5:$F5))*original_data!D5</f>
-        <v>13.335026670053338</v>
+        <v>26.676829268292682</v>
       </c>
       <c r="E5">
         <f>(100/SUM(original_data!$B5:$F5))*original_data!E5</f>
-        <v>11.91262382524765</v>
+        <v>23.831300813008131</v>
       </c>
       <c r="F5">
         <f>(100/SUM(original_data!$B5:$F5))*original_data!F5</f>
-        <v>50.012700025400051</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,23 +3891,23 @@
       </c>
       <c r="B6">
         <f>(100/SUM(original_data!$B6:$F6))*original_data!B6</f>
-        <v>11.379050489826678</v>
+        <v>22.752385735811149</v>
       </c>
       <c r="C6">
         <f>(100/SUM(original_data!$B6:$F6))*original_data!C6</f>
-        <v>12.308465209746297</v>
+        <v>24.610748367654445</v>
       </c>
       <c r="D6">
         <f>(100/SUM(original_data!$B6:$F6))*original_data!D6</f>
-        <v>12.358703843255464</v>
+        <v>24.711200401808135</v>
       </c>
       <c r="E6">
         <f>(100/SUM(original_data!$B6:$F6))*original_data!E6</f>
-        <v>13.966340115548856</v>
+        <v>27.925665494726264</v>
       </c>
       <c r="F6">
         <f>(100/SUM(original_data!$B6:$F6))*original_data!F6</f>
-        <v>49.987440341622701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,23 +3916,23 @@
       </c>
       <c r="B7">
         <f>(100/SUM(original_data!$B7:$F7))*original_data!B7</f>
-        <v>11.602484472049689</v>
+        <v>23.199205166418285</v>
       </c>
       <c r="C7">
         <f>(100/SUM(original_data!$B7:$F7))*original_data!C7</f>
-        <v>12.39751552795031</v>
+        <v>24.788872329855941</v>
       </c>
       <c r="D7">
         <f>(100/SUM(original_data!$B7:$F7))*original_data!D7</f>
-        <v>11.726708074534161</v>
+        <v>23.447590660705416</v>
       </c>
       <c r="E7">
         <f>(100/SUM(original_data!$B7:$F7))*original_data!E7</f>
-        <v>14.285714285714285</v>
+        <v>28.564331843020369</v>
       </c>
       <c r="F7">
         <f>(100/SUM(original_data!$B7:$F7))*original_data!F7</f>
-        <v>49.987577639751549</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,6 +4837,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1692,7 +4847,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F43" sqref="A1:F43"/>
+      <selection activeCell="F43" sqref="B43:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,26 +4858,26 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>1918</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="2">
         <f>(1918+1938)/2</f>
         <v>1928</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="2">
         <f>(1939+1959)/2</f>
         <v>1949</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <f>ROUND((1960+1975)/2,0)</f>
         <v>1968</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2">
         <f>ROUND((1976+2015)/2,2)</f>
         <v>1995.5</v>
       </c>
@@ -1743,9 +4898,6 @@
       <c r="E2">
         <v>4.01</v>
       </c>
-      <c r="F2">
-        <v>19.04</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1763,9 +4915,6 @@
       <c r="E3">
         <v>4.59</v>
       </c>
-      <c r="F3">
-        <v>19.260000000000002</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1783,9 +4932,6 @@
       <c r="E4">
         <v>4.29</v>
       </c>
-      <c r="F4">
-        <v>19.47</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1803,9 +4949,6 @@
       <c r="E5">
         <v>4.6900000000000004</v>
       </c>
-      <c r="F5">
-        <v>19.690000000000001</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1823,9 +4966,6 @@
       <c r="E6">
         <v>5.56</v>
       </c>
-      <c r="F6">
-        <v>19.899999999999999</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1842,9 +4982,6 @@
       </c>
       <c r="E7">
         <v>5.75</v>
-      </c>
-      <c r="F7">
-        <v>20.12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>